<commit_message>
Added remaining half of structural tests and tests for specific mutations in mutation testing, added before and after mutation html report
</commit_message>
<xml_diff>
--- a/Functional/Cause_effect_graph/Documents/Method1_test_table.xlsx
+++ b/Functional/Cause_effect_graph/Documents/Method1_test_table.xlsx
@@ -56,7 +56,7 @@
   </si>
   <si>
     <t xml:space="preserve">C1: new grade &lt; 0 or new grade &gt; 100
-C2: sem &lt; 0 or sem &gt; 2
+C2: sem &lt;= 0 or sem &gt; 2
 C3: subject length == 0
 C4: grade exists
 C5: replace is true</t>
@@ -286,7 +286,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>